<commit_message>
GSEA on X drivers
</commit_message>
<xml_diff>
--- a/data/cell-line-metadata.xlsx
+++ b/data/cell-line-metadata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smgroves/Documents/GitHub/Groves-CellSys2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7F48C5-352B-F74E-9372-616D92BA0574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183D30E4-B0FF-DC43-8B0B-9584E9EF4E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5160" yWindow="460" windowWidth="30680" windowHeight="21940" xr2:uid="{A884704C-6630-4B40-ABFD-E626947780C0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18000" windowHeight="21940" xr2:uid="{A884704C-6630-4B40-ABFD-E626947780C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="195">
   <si>
     <t>cell.line</t>
   </si>
@@ -596,6 +596,30 @@
   <si>
     <t>m</t>
   </si>
+  <si>
+    <t>Adh</t>
+  </si>
+  <si>
+    <t>Sus</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Suspension</t>
+  </si>
+  <si>
+    <t>Prior therapy</t>
+  </si>
+  <si>
+    <t>Non-A</t>
+  </si>
+  <si>
+    <t>Probability of getting 3/12 mixed if 3/80 non-N are mixed</t>
+  </si>
 </sst>
 </file>
 
@@ -728,6 +752,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF942093"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -737,6 +766,2164 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cell Line Growth Properties</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mixed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AA$11:$AE$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$12:$AE$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.3809523809523808E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E495-EB48-8D06-84A031581D3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adherent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AA$11:$AE$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$13:$AE$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.7619047619047616E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E495-EB48-8D06-84A031581D3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Suspension</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AA$11:$AE$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$14:$AE$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.69047619047619047</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27272727272727271</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E495-EB48-8D06-84A031581D3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unknown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AA$11:$AE$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$15:$AE$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.23809523809523808</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E495-EB48-8D06-84A031581D3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1475969199"/>
+        <c:axId val="1385059743"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1475969199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1385059743"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1385059743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1475969199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Prior Therapy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Yes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AA$40:$AB$40</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non-A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$41:$AB$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7816-D247-9AB5-1C8C3775ED06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AA$40:$AB$40</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non-A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$42:$AB$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7816-D247-9AB5-1C8C3775ED06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1404207519"/>
+        <c:axId val="1404772991"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1404207519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404772991"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1404772991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404207519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>218441</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>822818</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6702EF-6126-F54E-BFBF-152E2BDCBBC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>690880</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A69B41-63EF-C14A-A4B3-8FCA4E5C1C30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>44720</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>223593</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>146855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6F2FB8-B6FA-1A42-8E64-9E7619EB0D0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26410635" y="3946667"/>
+          <a:ext cx="2647324" cy="1137089"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1036,11 +3223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B41ADB5-C4D7-094D-919D-E3C4D59CD31A}">
-  <dimension ref="A1:V996"/>
+  <dimension ref="A1:AE996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="142" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1055,7 +3242,7 @@
     <col min="21" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,7 +3308,7 @@
       </c>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1168,7 +3355,7 @@
       </c>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1215,7 +3402,7 @@
       </c>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1260,7 +3447,7 @@
       </c>
       <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>149</v>
       </c>
@@ -1270,7 +3457,9 @@
       <c r="C5" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>51</v>
       </c>
@@ -1301,8 +3490,23 @@
         <v>171</v>
       </c>
       <c r="V5" s="4"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA5" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1312,7 +3516,9 @@
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1345,8 +3551,26 @@
         <v>171</v>
       </c>
       <c r="V6" s="4"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z6" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>11</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1393,8 +3617,26 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z7" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>29</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>6</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1434,8 +3676,26 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z8" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>143</v>
       </c>
@@ -1445,7 +3705,9 @@
       <c r="C9" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>59</v>
       </c>
@@ -1476,8 +3738,26 @@
         <v>171</v>
       </c>
       <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z9" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1527,7 +3807,7 @@
       </c>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
@@ -1537,7 +3817,9 @@
       <c r="C11" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1574,8 +3856,23 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AA11" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE11" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>159</v>
       </c>
@@ -1616,8 +3913,26 @@
         <v>171</v>
       </c>
       <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z12" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>2.3809523809523808E-2</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1672,8 +3987,26 @@
         <v>171</v>
       </c>
       <c r="V13" s="4"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z13" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AB13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AE13" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1683,7 +4016,9 @@
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1714,8 +4049,26 @@
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z14" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>0.69047619047619047</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>137</v>
       </c>
@@ -1744,8 +4097,26 @@
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z15" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA15" s="5">
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="AC15" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AE15" s="5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>61</v>
       </c>
@@ -1775,7 +4146,7 @@
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>138</v>
       </c>
@@ -1805,7 +4176,7 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>84</v>
       </c>
@@ -1834,8 +4205,11 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="AD18" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1845,7 +4219,9 @@
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1883,7 +4259,7 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1933,7 +4309,7 @@
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1943,7 +4319,9 @@
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1979,7 +4357,7 @@
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>144</v>
       </c>
@@ -1989,7 +4367,9 @@
       <c r="C22" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2009,7 +4389,7 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -2019,7 +4399,9 @@
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2055,7 +4437,7 @@
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>169</v>
       </c>
@@ -2085,7 +4467,7 @@
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>145</v>
       </c>
@@ -2095,7 +4477,9 @@
       <c r="C25" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2115,7 +4499,7 @@
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -2125,7 +4509,9 @@
       <c r="C26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2157,7 +4543,7 @@
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>147</v>
       </c>
@@ -2167,7 +4553,9 @@
       <c r="C27" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2187,7 +4575,7 @@
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -2197,7 +4585,9 @@
       <c r="C28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E28" s="4" t="s">
         <v>51</v>
       </c>
@@ -2229,7 +4619,7 @@
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>150</v>
       </c>
@@ -2259,7 +4649,7 @@
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2269,7 +4659,9 @@
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2305,7 +4697,7 @@
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>151</v>
       </c>
@@ -2315,7 +4707,9 @@
       <c r="C31" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2335,7 +4729,7 @@
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>152</v>
       </c>
@@ -2365,7 +4759,7 @@
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -2417,7 +4811,7 @@
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
@@ -2427,7 +4821,9 @@
       <c r="C34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E34" s="4" t="s">
         <v>51</v>
       </c>
@@ -2457,7 +4853,7 @@
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
@@ -2467,7 +4863,9 @@
       <c r="C35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>21</v>
       </c>
@@ -2496,8 +4894,26 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z35" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA35" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB35" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC35" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD35" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE35" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>154</v>
       </c>
@@ -2507,7 +4923,9 @@
       <c r="C36" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2526,8 +4944,26 @@
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA36" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB36" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC36" s="5">
+        <v>7</v>
+      </c>
+      <c r="AD36" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE36" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>155</v>
       </c>
@@ -2537,7 +4973,9 @@
       <c r="C37" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2556,8 +4994,26 @@
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA37" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB37" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC37" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>158</v>
       </c>
@@ -2587,7 +5043,7 @@
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>163</v>
       </c>
@@ -2597,7 +5053,9 @@
       <c r="C39" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2617,7 +5075,7 @@
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>165</v>
       </c>
@@ -2646,8 +5104,17 @@
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z40" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA40" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB40" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>141</v>
       </c>
@@ -2678,8 +5145,17 @@
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA41" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB41" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>166</v>
       </c>
@@ -2689,7 +5165,9 @@
       <c r="C42" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2708,8 +5186,17 @@
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z42" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA42" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB42" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>81</v>
       </c>
@@ -2751,7 +5238,7 @@
       </c>
       <c r="V43" s="4"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>102</v>
       </c>
@@ -2800,7 +5287,7 @@
       </c>
       <c r="V44" s="4"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>157</v>
       </c>
@@ -2810,7 +5297,9 @@
       <c r="C45" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="4"/>
+      <c r="D45" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
         <v>93</v>
@@ -2840,7 +5329,7 @@
       </c>
       <c r="V45" s="4"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>96</v>
       </c>
@@ -2887,7 +5376,7 @@
       </c>
       <c r="V46" s="4"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>86</v>
       </c>
@@ -2936,7 +5425,7 @@
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -3211,7 +5700,9 @@
       <c r="C54" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D54" s="4"/>
+      <c r="D54" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -3271,7 +5762,9 @@
       <c r="C56" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -3377,7 +5870,9 @@
       <c r="C59" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D59" s="4"/>
+      <c r="D59" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -3407,7 +5902,9 @@
       <c r="C60" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E60" s="2" t="s">
         <v>21</v>
       </c>
@@ -3455,7 +5952,9 @@
       <c r="C61" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -3485,7 +5984,9 @@
       <c r="C62" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D62" s="4"/>
+      <c r="D62" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -3515,7 +6016,9 @@
       <c r="C63" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D63" s="4"/>
+      <c r="D63" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -3545,7 +6048,9 @@
       <c r="C64" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D64" s="4"/>
+      <c r="D64" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4" t="s">
         <v>26</v>
@@ -3721,7 +6226,9 @@
       <c r="C68" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4" t="s">
         <v>22</v>
@@ -3916,7 +6423,7 @@
         <v>20</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>21</v>
@@ -26536,5 +29043,6 @@
     <hyperlink ref="U46" r:id="rId7" xr:uid="{9DDDCE8E-BBBE-9F42-A9DA-137CD6DF994F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>